<commit_message>
fix bug, final!!oh yeah!
</commit_message>
<xml_diff>
--- a/doc/pr3_report/memorytop-IO-signal.xlsx
+++ b/doc/pr3_report/memorytop-IO-signal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amber\mygit\makecomputer\doc\pr3_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\release\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -218,7 +218,41 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -229,6 +263,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A1:I12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:I12"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="信号" dataDxfId="10"/>
+    <tableColumn id="2" name="BOOT_FLASH" dataDxfId="9"/>
+    <tableColumn id="3" name="BOOT_RAM1" dataDxfId="8"/>
+    <tableColumn id="4" name="BOOT_RAM2" dataDxfId="7"/>
+    <tableColumn id="5" name="BOOT_READY" dataDxfId="6"/>
+    <tableColumn id="6" name="READ1" dataDxfId="5"/>
+    <tableColumn id="7" name="IDEL1" dataDxfId="4"/>
+    <tableColumn id="8" name="RW1" dataDxfId="3"/>
+    <tableColumn id="9" name="IDEL2" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,10 +549,15 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I12"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="3" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="12.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
@@ -854,5 +911,8 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>